<commit_message>
Add video and sounds
</commit_message>
<xml_diff>
--- a/Documentation/模块分组.xlsx
+++ b/Documentation/模块分组.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13725" windowHeight="12390"/>
+    <workbookView windowWidth="21720" windowHeight="10335"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>序号</t>
   </si>
@@ -133,6 +133,15 @@
   </si>
   <si>
     <t>SIM</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>Sound</t>
+  </si>
+  <si>
+    <t>王世浩、曹燃</t>
   </si>
 </sst>
 </file>
@@ -140,12 +149,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,96 +172,57 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -291,12 +261,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
@@ -305,7 +299,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -320,187 +322,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -530,6 +532,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -546,26 +563,33 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -585,30 +609,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -620,9 +620,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -631,159 +633,156 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1137,15 +1136,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
     <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="16.55" customWidth="1"/>
     <col min="6" max="6" width="6.25" customWidth="1"/>
     <col min="7" max="7" width="26.5" customWidth="1"/>
   </cols>
@@ -1168,13 +1168,13 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1182,13 +1182,13 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1196,13 +1196,13 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1210,13 +1210,13 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1224,13 +1224,13 @@
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1238,13 +1238,13 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1252,13 +1252,13 @@
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1266,13 +1266,13 @@
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1280,13 +1280,13 @@
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1294,13 +1294,13 @@
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1308,13 +1308,13 @@
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1322,13 +1322,13 @@
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1336,13 +1336,13 @@
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1350,13 +1350,13 @@
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1364,13 +1364,13 @@
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1378,14 +1378,42 @@
       <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>